<commit_message>
few more exploratory analyses
</commit_message>
<xml_diff>
--- a/data/quick_analysis.xlsx
+++ b/data/quick_analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ffce2ed1cf6c3ec/Documents/University/Year Four/CITS4001 Thesis/honours/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\OneDrive\Documents\University\Year Four\CITS4001 Thesis\honours\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>2016-Sep-09</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>2013-Dec-xx</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>milestones</t>
+  </si>
+  <si>
+    <t>objects</t>
+  </si>
+  <si>
+    <t>offices</t>
+  </si>
+  <si>
+    <t>relationships</t>
   </si>
 </sst>
 </file>
@@ -143,17 +161,45 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -462,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I24"/>
+  <dimension ref="B2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,28 +522,33 @@
     <col min="5" max="5" width="11.21875" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.44140625" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -517,13 +568,16 @@
         <v>114949</v>
       </c>
       <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>31679</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -545,11 +599,14 @@
       <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="I4">
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4">
         <v>4651</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -559,7 +616,7 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
@@ -568,18 +625,18 @@
       <c r="G5">
         <v>66368</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>25</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>17727</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D6" t="s">
@@ -597,11 +654,14 @@
       <c r="H6" t="s">
         <v>17</v>
       </c>
-      <c r="I6">
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6">
         <v>34226</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -614,8 +674,11 @@
       <c r="E7">
         <v>7001</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -629,7 +692,29 @@
         <v>47632</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>545451</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>4954</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>9</v>
       </c>
@@ -637,7 +722,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>18</v>
       </c>
@@ -645,7 +730,7 @@
         <v>942542</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>19</v>
       </c>
@@ -653,7 +738,7 @@
         <v>6080</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>20</v>
       </c>
@@ -661,7 +746,7 @@
         <v>259448</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>21</v>
       </c>
@@ -669,83 +754,93 @@
         <v>470783</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16">
-        <v>545451</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+        <v>290227</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>290227</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+        <v>502358</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E18">
-        <v>502358</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+        <v>109569</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E19">
-        <v>109569</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+        <v>7075</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <v>7075</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+        <v>251337</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E21">
-        <v>251337</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22">
-        <v>4954</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23">
         <v>40994</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F24" t="s">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
         <v>24</v>
       </c>
-      <c r="G24">
+      <c r="G22">
         <v>2213</v>
       </c>
     </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>